<commit_message>
TEst statement json files were created for each broker
</commit_message>
<xml_diff>
--- a/tests/test_data/psb.xlsx
+++ b/tests/test_data/psb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="243">
   <si>
     <t xml:space="preserve">Почтовый адрес: 109052, Россия, г. Москва, ул. Смирновская, д.10, стр.22</t>
   </si>
@@ -712,13 +712,16 @@
     <t xml:space="preserve">Валюта Выплаты</t>
   </si>
   <si>
-    <t xml:space="preserve">АО "Нижнекамскнефтехим" (НКНХ) ПАО, выпуск 02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU0009100507</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-02-00096-A</t>
+    <t xml:space="preserve">28.04.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПАО Московская Биржа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU000A0JR4A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-05-08443-H</t>
   </si>
   <si>
     <t xml:space="preserve">Дата составления отчета: </t>
@@ -1044,7 +1047,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="90">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1363,14 +1366,6 @@
     </xf>
     <xf numFmtId="167" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1433,11 +1428,11 @@
   </sheetPr>
   <dimension ref="A1:AN1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K122" activeCellId="0" sqref="K122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -4360,9 +4355,9 @@
       <c r="I80" s="76"/>
       <c r="J80" s="76"/>
       <c r="K80" s="76"/>
-      <c r="L80" s="80"/>
-      <c r="M80" s="80"/>
-      <c r="N80" s="81"/>
+      <c r="L80" s="74"/>
+      <c r="M80" s="74"/>
+      <c r="N80" s="50"/>
       <c r="O80" s="75"/>
       <c r="P80" s="75"/>
     </row>
@@ -4423,10 +4418,10 @@
       <c r="B82" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="C82" s="82" t="s">
+      <c r="C82" s="80" t="s">
         <v>163</v>
       </c>
-      <c r="D82" s="82"/>
+      <c r="D82" s="80"/>
       <c r="E82" s="68" t="s">
         <v>164</v>
       </c>
@@ -4543,7 +4538,7 @@
       <c r="L84" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="M84" s="83"/>
+      <c r="M84" s="81"/>
       <c r="N84" s="53" t="n">
         <v>2009.8</v>
       </c>
@@ -4584,7 +4579,7 @@
       <c r="L85" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="M85" s="83"/>
+      <c r="M85" s="81"/>
       <c r="N85" s="53" t="n">
         <v>-1.6</v>
       </c>
@@ -4625,7 +4620,7 @@
       <c r="L86" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="M86" s="83"/>
+      <c r="M86" s="81"/>
       <c r="N86" s="53" t="n">
         <v>1005.7</v>
       </c>
@@ -4649,43 +4644,43 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="84" t="s">
+      <c r="B87" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="C87" s="84"/>
-      <c r="D87" s="84"/>
-      <c r="E87" s="84"/>
-      <c r="F87" s="84"/>
-      <c r="G87" s="84"/>
-      <c r="H87" s="84"/>
-      <c r="I87" s="84"/>
-      <c r="J87" s="84"/>
-      <c r="K87" s="85" t="n">
+      <c r="C87" s="82"/>
+      <c r="D87" s="82"/>
+      <c r="E87" s="82"/>
+      <c r="F87" s="82"/>
+      <c r="G87" s="82"/>
+      <c r="H87" s="82"/>
+      <c r="I87" s="82"/>
+      <c r="J87" s="82"/>
+      <c r="K87" s="83" t="n">
         <v>1</v>
       </c>
-      <c r="L87" s="84" t="s">
+      <c r="L87" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="M87" s="86"/>
-      <c r="N87" s="87" t="n">
+      <c r="M87" s="84"/>
+      <c r="N87" s="85" t="n">
         <v>1004.1</v>
       </c>
-      <c r="O87" s="87" t="n">
+      <c r="O87" s="85" t="n">
         <v>17.03</v>
       </c>
-      <c r="P87" s="87" t="n">
+      <c r="P87" s="85" t="n">
         <v>0.04</v>
       </c>
-      <c r="Q87" s="87" t="n">
+      <c r="Q87" s="85" t="n">
         <v>-0.04</v>
       </c>
-      <c r="R87" s="87" t="n">
+      <c r="R87" s="85" t="n">
         <v>-0.02</v>
       </c>
-      <c r="S87" s="84" t="s">
+      <c r="S87" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="T87" s="87" t="n">
+      <c r="T87" s="85" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -4849,7 +4844,7 @@
       <c r="M92" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="N92" s="83"/>
+      <c r="N92" s="81"/>
       <c r="O92" s="53" t="n">
         <v>9876.5</v>
       </c>
@@ -4891,7 +4886,7 @@
       <c r="M93" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="N93" s="83"/>
+      <c r="N93" s="81"/>
       <c r="O93" s="53" t="n">
         <v>0</v>
       </c>
@@ -4933,7 +4928,7 @@
       <c r="M94" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="N94" s="83"/>
+      <c r="N94" s="81"/>
       <c r="O94" s="53" t="n">
         <v>9876.5</v>
       </c>
@@ -4957,44 +4952,44 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="84" t="s">
+      <c r="B95" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="C95" s="84"/>
-      <c r="D95" s="84"/>
-      <c r="E95" s="84"/>
-      <c r="F95" s="84"/>
-      <c r="G95" s="84"/>
-      <c r="H95" s="84"/>
-      <c r="I95" s="84"/>
-      <c r="J95" s="84"/>
-      <c r="K95" s="84"/>
-      <c r="L95" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="M95" s="84" t="s">
+      <c r="C95" s="82"/>
+      <c r="D95" s="82"/>
+      <c r="E95" s="82"/>
+      <c r="F95" s="82"/>
+      <c r="G95" s="82"/>
+      <c r="H95" s="82"/>
+      <c r="I95" s="82"/>
+      <c r="J95" s="82"/>
+      <c r="K95" s="82"/>
+      <c r="L95" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="N95" s="86"/>
-      <c r="O95" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="P95" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q95" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="R95" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="S95" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="T95" s="84" t="s">
+      <c r="N95" s="84"/>
+      <c r="O95" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P95" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="R95" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T95" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="U95" s="87" t="n">
+      <c r="U95" s="85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5018,9 +5013,9 @@
       <c r="K97" s="76"/>
       <c r="L97" s="76"/>
       <c r="M97" s="76"/>
-      <c r="N97" s="80"/>
-      <c r="O97" s="80"/>
-      <c r="P97" s="81"/>
+      <c r="N97" s="74"/>
+      <c r="O97" s="74"/>
+      <c r="P97" s="50"/>
       <c r="Q97" s="75"/>
       <c r="R97" s="75"/>
     </row>
@@ -5159,7 +5154,7 @@
       <c r="M100" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="N100" s="83"/>
+      <c r="N100" s="81"/>
       <c r="O100" s="53" t="n">
         <v>15321</v>
       </c>
@@ -5201,7 +5196,7 @@
       <c r="M101" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="N101" s="83"/>
+      <c r="N101" s="81"/>
       <c r="O101" s="53" t="n">
         <v>-15321</v>
       </c>
@@ -5243,7 +5238,7 @@
       <c r="M102" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="N102" s="83"/>
+      <c r="N102" s="81"/>
       <c r="O102" s="53" t="n">
         <v>15321</v>
       </c>
@@ -5267,44 +5262,44 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="84" t="s">
+      <c r="B103" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="C103" s="84"/>
-      <c r="D103" s="84"/>
-      <c r="E103" s="84"/>
-      <c r="F103" s="84"/>
-      <c r="G103" s="84"/>
-      <c r="H103" s="84"/>
-      <c r="I103" s="84"/>
-      <c r="J103" s="84"/>
-      <c r="K103" s="84"/>
-      <c r="L103" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="M103" s="84" t="s">
+      <c r="C103" s="82"/>
+      <c r="D103" s="82"/>
+      <c r="E103" s="82"/>
+      <c r="F103" s="82"/>
+      <c r="G103" s="82"/>
+      <c r="H103" s="82"/>
+      <c r="I103" s="82"/>
+      <c r="J103" s="82"/>
+      <c r="K103" s="82"/>
+      <c r="L103" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="N103" s="86"/>
-      <c r="O103" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="P103" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q103" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="R103" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="S103" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="T103" s="84" t="s">
+      <c r="N103" s="84"/>
+      <c r="O103" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P103" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="R103" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="S103" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T103" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="U103" s="87" t="n">
+      <c r="U103" s="85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5330,7 +5325,7 @@
       <c r="A106" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="B106" s="88" t="s">
+      <c r="B106" s="86" t="s">
         <v>195</v>
       </c>
       <c r="C106" s="71" t="s">
@@ -5357,25 +5352,25 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="88"/>
-      <c r="C107" s="88"/>
-      <c r="D107" s="88"/>
-      <c r="E107" s="88"/>
-      <c r="F107" s="88"/>
-      <c r="G107" s="88"/>
-      <c r="H107" s="88" t="s">
+      <c r="B107" s="86"/>
+      <c r="C107" s="86"/>
+      <c r="D107" s="86"/>
+      <c r="E107" s="86"/>
+      <c r="F107" s="86"/>
+      <c r="G107" s="86"/>
+      <c r="H107" s="86" t="s">
         <v>202</v>
       </c>
-      <c r="I107" s="88" t="s">
+      <c r="I107" s="86" t="s">
         <v>203</v>
       </c>
-      <c r="J107" s="88" t="s">
+      <c r="J107" s="86" t="s">
         <v>204</v>
       </c>
-      <c r="K107" s="88" t="s">
+      <c r="K107" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="L107" s="88" t="s">
+      <c r="L107" s="86" t="s">
         <v>206</v>
       </c>
     </row>
@@ -5443,29 +5438,29 @@
       <c r="A110" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="B110" s="89" t="s">
+      <c r="B110" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C110" s="89" t="s">
+      <c r="C110" s="87" t="s">
         <v>212</v>
       </c>
-      <c r="D110" s="89"/>
-      <c r="E110" s="89"/>
-      <c r="F110" s="89"/>
-      <c r="G110" s="89"/>
-      <c r="H110" s="90" t="n">
+      <c r="D110" s="87"/>
+      <c r="E110" s="87"/>
+      <c r="F110" s="87"/>
+      <c r="G110" s="87"/>
+      <c r="H110" s="88" t="n">
         <v>310.85</v>
       </c>
-      <c r="I110" s="90" t="n">
+      <c r="I110" s="88" t="n">
         <v>18585.98</v>
       </c>
-      <c r="J110" s="90" t="n">
+      <c r="J110" s="88" t="n">
         <v>18585.98</v>
       </c>
-      <c r="K110" s="90" t="n">
+      <c r="K110" s="88" t="n">
         <v>18585.98</v>
       </c>
-      <c r="L110" s="90" t="n">
+      <c r="L110" s="88" t="n">
         <v>18585.98</v>
       </c>
     </row>
@@ -5493,17 +5488,17 @@
       <c r="A113" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="B113" s="88" t="s">
+      <c r="B113" s="86" t="s">
         <v>216</v>
       </c>
-      <c r="C113" s="88"/>
-      <c r="D113" s="88"/>
-      <c r="E113" s="88" t="s">
+      <c r="C113" s="86"/>
+      <c r="D113" s="86"/>
+      <c r="E113" s="86" t="s">
         <v>196</v>
       </c>
-      <c r="F113" s="88"/>
-      <c r="G113" s="88"/>
-      <c r="H113" s="88"/>
+      <c r="F113" s="86"/>
+      <c r="G113" s="86"/>
+      <c r="H113" s="86"/>
       <c r="I113" s="71" t="s">
         <v>197</v>
       </c>
@@ -5521,26 +5516,26 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="34.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="88"/>
-      <c r="C114" s="88"/>
-      <c r="D114" s="88"/>
-      <c r="E114" s="88"/>
-      <c r="F114" s="88"/>
-      <c r="G114" s="88"/>
-      <c r="H114" s="88"/>
-      <c r="I114" s="88" t="s">
+      <c r="B114" s="86"/>
+      <c r="C114" s="86"/>
+      <c r="D114" s="86"/>
+      <c r="E114" s="86"/>
+      <c r="F114" s="86"/>
+      <c r="G114" s="86"/>
+      <c r="H114" s="86"/>
+      <c r="I114" s="86" t="s">
         <v>202</v>
       </c>
-      <c r="J114" s="88" t="s">
+      <c r="J114" s="86" t="s">
         <v>203</v>
       </c>
-      <c r="K114" s="88" t="s">
+      <c r="K114" s="86" t="s">
         <v>204</v>
       </c>
-      <c r="L114" s="88" t="s">
+      <c r="L114" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="M114" s="88" t="s">
+      <c r="M114" s="86" t="s">
         <v>206</v>
       </c>
     </row>
@@ -5610,30 +5605,30 @@
       <c r="A117" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="B117" s="89" t="s">
+      <c r="B117" s="87" t="s">
         <v>218</v>
       </c>
-      <c r="C117" s="89"/>
-      <c r="D117" s="89"/>
-      <c r="E117" s="89" t="s">
+      <c r="C117" s="87"/>
+      <c r="D117" s="87"/>
+      <c r="E117" s="87" t="s">
         <v>212</v>
       </c>
-      <c r="F117" s="89"/>
-      <c r="G117" s="89"/>
-      <c r="H117" s="89"/>
-      <c r="I117" s="85" t="n">
+      <c r="F117" s="87"/>
+      <c r="G117" s="87"/>
+      <c r="H117" s="87"/>
+      <c r="I117" s="83" t="n">
         <v>3</v>
       </c>
-      <c r="J117" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="K117" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="L117" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="M117" s="85" t="n">
+      <c r="J117" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="K117" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="M117" s="83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5696,40 +5691,40 @@
     </row>
     <row r="121" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="72" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="C121" s="68" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D121" s="68"/>
       <c r="E121" s="68"/>
       <c r="F121" s="68"/>
       <c r="G121" s="68" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H121" s="68" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I121" s="77" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="J121" s="68" t="s">
         <v>14</v>
       </c>
       <c r="K121" s="78" t="n">
-        <v>0.73</v>
+        <v>141.75</v>
       </c>
       <c r="L121" s="61" t="n">
-        <v>29.2</v>
+        <v>1417.5</v>
       </c>
       <c r="M121" s="61" t="n">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="N121" s="61" t="s">
         <v>14</v>
       </c>
       <c r="O121" s="61" t="n">
-        <v>25.2</v>
+        <v>1233.5</v>
       </c>
       <c r="P121" s="68" t="s">
         <v>14</v>
@@ -5738,44 +5733,44 @@
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="34"/>
       <c r="B130" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C130" s="34"/>
       <c r="D130" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="34"/>
       <c r="B132" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C132" s="38"/>
       <c r="D132" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E132" s="11"/>
       <c r="F132" s="34"/>
       <c r="G132" s="34"/>
       <c r="H132" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I132" s="34"/>
       <c r="J132" s="34"/>
       <c r="K132" s="34"/>
       <c r="L132" s="11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M132" s="34"/>
       <c r="N132" s="34"/>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B133" s="23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C133" s="23" t="n">
         <v>82</v>
@@ -5784,23 +5779,23 @@
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="B135" s="91" t="s">
         <v>241</v>
       </c>
-      <c r="C135" s="91"/>
-      <c r="D135" s="91"/>
-      <c r="E135" s="91"/>
-      <c r="F135" s="91"/>
-      <c r="G135" s="91"/>
-      <c r="H135" s="91"/>
-      <c r="I135" s="91"/>
-      <c r="J135" s="91"/>
-      <c r="K135" s="91"/>
-      <c r="L135" s="91"/>
-      <c r="M135" s="91"/>
-      <c r="N135" s="91"/>
+      <c r="B135" s="89" t="s">
+        <v>242</v>
+      </c>
+      <c r="C135" s="89"/>
+      <c r="D135" s="89"/>
+      <c r="E135" s="89"/>
+      <c r="F135" s="89"/>
+      <c r="G135" s="89"/>
+      <c r="H135" s="89"/>
+      <c r="I135" s="89"/>
+      <c r="J135" s="89"/>
+      <c r="K135" s="89"/>
+      <c r="L135" s="89"/>
+      <c r="M135" s="89"/>
+      <c r="N135" s="89"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Class PSB_Broker was replaced with StatementPSB (based on StatementXLS) in order to load statements via intermediate JSON validation. Test set was updated.
</commit_message>
<xml_diff>
--- a/tests/test_data/psb.xlsx
+++ b/tests/test_data/psb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="258">
   <si>
     <t xml:space="preserve">Почтовый адрес: 109052, Россия, г. Москва, ул. Смирновская, д.10, стр.22</t>
   </si>
@@ -382,6 +382,15 @@
     <t xml:space="preserve">Дивиденды АО "Нижнекамскнефтехим" (НКНХ) ПАО, выпуск 02 ISIN RU0009100507</t>
   </si>
   <si>
+    <t xml:space="preserve">09.04.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.05.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Списано со счета</t>
+  </si>
+  <si>
     <t xml:space="preserve">Портфель на конец дня на биржевом рынке</t>
   </si>
   <si>
@@ -688,12 +697,54 @@
     <t xml:space="preserve">КонецТаблТрОбЦБ</t>
   </si>
   <si>
+    <t xml:space="preserve">Погашение купонов и ЦБ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата операции</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вид операции</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регистрационный номер ЦБ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кол-во ЦБ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номинал сумма амортизации долга</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумма удержанного налога, руб.*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фактическая сумма выплаты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Валюта Выплаты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Состояние</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.03.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Погашение купона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТинькоффБ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выплачено</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Налог удерживается с рублевого брокерского счета и указывается в поле "Налог удержанный" в дату фактического списания, только при выплате доходов, выраженных (номинированных) в иностранной  валюте</t>
+  </si>
+  <si>
     <t xml:space="preserve">Выплата дивидендов</t>
   </si>
   <si>
-    <t xml:space="preserve">Дата операции</t>
-  </si>
-  <si>
     <t xml:space="preserve">Размер дивидендов на 1 акцию</t>
   </si>
   <si>
@@ -704,12 +755,6 @@
   </si>
   <si>
     <t xml:space="preserve">Валюта удержания налога </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фактическая сумма выплаты</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Валюта Выплаты</t>
   </si>
   <si>
     <t xml:space="preserve">28.04.2021</t>
@@ -1047,7 +1092,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1402,6 +1447,14 @@
     </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1426,10 +1479,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AN1048576"/>
+  <dimension ref="A1:AN142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K122" activeCellId="0" sqref="K122"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D73" activeCellId="0" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4077,189 +4130,129 @@
       <c r="K70" s="68"/>
       <c r="L70" s="68"/>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="76" t="s">
+    <row r="71" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B71" s="72" t="s">
         <v>120</v>
       </c>
-      <c r="C72" s="76"/>
-      <c r="D72" s="76"/>
-      <c r="E72" s="76"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="50"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="75"/>
-    </row>
-    <row r="73" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="23" t="s">
+      <c r="C71" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="61" t="n">
+        <v>5214.84</v>
+      </c>
+      <c r="E71" s="61"/>
+      <c r="F71" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="G71" s="68"/>
+      <c r="H71" s="68"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="68"/>
+      <c r="K71" s="68"/>
+      <c r="L71" s="68"/>
+    </row>
+    <row r="72" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B72" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="70" t="s">
+      <c r="C72" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="61" t="n">
+        <v>-2385.14</v>
+      </c>
+      <c r="E72" s="61"/>
+      <c r="F72" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="C73" s="70"/>
-      <c r="D73" s="70"/>
-      <c r="E73" s="71" t="s">
+      <c r="G72" s="68"/>
+      <c r="H72" s="68"/>
+      <c r="I72" s="68"/>
+      <c r="J72" s="68"/>
+      <c r="K72" s="68"/>
+      <c r="L72" s="68"/>
+    </row>
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="F73" s="71" t="s">
+      <c r="C74" s="76"/>
+      <c r="D74" s="76"/>
+      <c r="E74" s="76"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="50"/>
+      <c r="H74" s="75"/>
+      <c r="I74" s="75"/>
+    </row>
+    <row r="75" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="G73" s="71" t="s">
+      <c r="B75" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="H73" s="71" t="s">
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="F75" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="G75" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="H75" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="I73" s="71" t="s">
+      <c r="I75" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="J73" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="K73" s="71" t="s">
-        <v>127</v>
-      </c>
-      <c r="L73" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="M73" s="71" t="s">
+      <c r="J75" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="N73" s="71" t="s">
+      <c r="K75" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="O73" s="71" t="s">
+      <c r="L75" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="P73" s="71" t="s">
+      <c r="M75" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="Q73" s="71" t="s">
+      <c r="N75" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="R73" s="71" t="s">
+      <c r="O75" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="S73" s="71" t="s">
+      <c r="P75" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q75" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="R75" s="71" t="s">
+        <v>137</v>
+      </c>
+      <c r="S75" s="71" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="C74" s="72"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="68" t="s">
-        <v>136</v>
-      </c>
-      <c r="F74" s="68" t="s">
-        <v>137</v>
-      </c>
-      <c r="G74" s="77" t="n">
-        <v>20</v>
-      </c>
-      <c r="H74" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="I74" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="J74" s="77" t="n">
-        <v>20</v>
-      </c>
-      <c r="K74" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="L74" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="M74" s="78" t="n">
-        <v>65.9</v>
-      </c>
-      <c r="N74" s="61" t="n">
-        <v>1318</v>
-      </c>
-      <c r="O74" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="P74" s="78" t="n">
-        <v>66</v>
-      </c>
-      <c r="Q74" s="61" t="n">
-        <v>1320</v>
-      </c>
-      <c r="R74" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="S74" s="77" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="72" t="s">
+    <row r="76" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B76" s="72" t="s">
         <v>138</v>
-      </c>
-      <c r="C75" s="72"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="68" t="s">
-        <v>139</v>
-      </c>
-      <c r="F75" s="68"/>
-      <c r="G75" s="77" t="n">
-        <v>10</v>
-      </c>
-      <c r="H75" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="I75" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="J75" s="77" t="n">
-        <v>10</v>
-      </c>
-      <c r="K75" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="L75" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="M75" s="78" t="n">
-        <v>891.6</v>
-      </c>
-      <c r="N75" s="61" t="n">
-        <v>8916</v>
-      </c>
-      <c r="O75" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="P75" s="78" t="n">
-        <v>900</v>
-      </c>
-      <c r="Q75" s="61" t="n">
-        <v>9000</v>
-      </c>
-      <c r="R75" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="S75" s="77" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="72" t="s">
-        <v>140</v>
       </c>
       <c r="C76" s="72"/>
       <c r="D76" s="72"/>
       <c r="E76" s="68" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F76" s="68" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G76" s="77" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H76" s="77" t="n">
         <v>0</v>
@@ -4268,7 +4261,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="77" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="K76" s="68" t="s">
         <v>14</v>
@@ -4277,334 +4270,354 @@
         <v>14</v>
       </c>
       <c r="M76" s="78" t="n">
+        <v>65.9</v>
+      </c>
+      <c r="N76" s="61" t="n">
+        <v>1318</v>
+      </c>
+      <c r="O76" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" s="78" t="n">
+        <v>66</v>
+      </c>
+      <c r="Q76" s="61" t="n">
+        <v>1320</v>
+      </c>
+      <c r="R76" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="S76" s="77" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B77" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" s="72"/>
+      <c r="D77" s="72"/>
+      <c r="E77" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="F77" s="68"/>
+      <c r="G77" s="77" t="n">
+        <v>10</v>
+      </c>
+      <c r="H77" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" s="77" t="n">
+        <v>10</v>
+      </c>
+      <c r="K77" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="L77" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="M77" s="78" t="n">
+        <v>891.6</v>
+      </c>
+      <c r="N77" s="61" t="n">
+        <v>8916</v>
+      </c>
+      <c r="O77" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P77" s="78" t="n">
+        <v>900</v>
+      </c>
+      <c r="Q77" s="61" t="n">
+        <v>9000</v>
+      </c>
+      <c r="R77" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" s="77" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B78" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="C78" s="72"/>
+      <c r="D78" s="72"/>
+      <c r="E78" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="F78" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="G78" s="77" t="n">
+        <v>50</v>
+      </c>
+      <c r="H78" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="77" t="n">
+        <v>50</v>
+      </c>
+      <c r="K78" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="L78" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="M78" s="78" t="n">
         <v>100.05</v>
       </c>
-      <c r="N76" s="61" t="n">
+      <c r="N78" s="61" t="n">
         <v>50025</v>
       </c>
-      <c r="O76" s="61" t="n">
-        <v>33</v>
-      </c>
-      <c r="P76" s="78" t="n">
+      <c r="O78" s="61" t="n">
+        <v>33</v>
+      </c>
+      <c r="P78" s="78" t="n">
         <v>100.09</v>
       </c>
-      <c r="Q76" s="61" t="n">
+      <c r="Q78" s="61" t="n">
         <v>50045</v>
       </c>
-      <c r="R76" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="S76" s="77" t="n">
+      <c r="R78" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" s="77" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="B77" s="73" t="s">
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B79" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="C79" s="73"/>
+      <c r="D79" s="73"/>
+      <c r="E79" s="53"/>
+      <c r="F79" s="53"/>
+      <c r="G79" s="79" t="n">
+        <v>80</v>
+      </c>
+      <c r="H79" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" s="79" t="n">
+        <v>80</v>
+      </c>
+      <c r="K79" s="73"/>
+      <c r="L79" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="M79" s="53"/>
+      <c r="N79" s="53" t="n">
+        <v>60259</v>
+      </c>
+      <c r="O79" s="53" t="n">
+        <v>33</v>
+      </c>
+      <c r="P79" s="53"/>
+      <c r="Q79" s="53"/>
+      <c r="R79" s="53"/>
+      <c r="S79" s="53"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="C82" s="76"/>
+      <c r="D82" s="76"/>
+      <c r="E82" s="76"/>
+      <c r="F82" s="76"/>
+      <c r="G82" s="76"/>
+      <c r="H82" s="76"/>
+      <c r="I82" s="76"/>
+      <c r="J82" s="76"/>
+      <c r="K82" s="76"/>
+      <c r="L82" s="74"/>
+      <c r="M82" s="74"/>
+      <c r="N82" s="50"/>
+      <c r="O82" s="75"/>
+      <c r="P82" s="75"/>
+    </row>
+    <row r="83" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B83" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="C83" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" s="71"/>
+      <c r="E83" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="F83" s="71"/>
+      <c r="G83" s="71"/>
+      <c r="H83" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="I83" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="J83" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="K83" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="L83" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="M83" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="N83" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="O83" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="P83" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q83" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="R83" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="S83" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="T83" s="71" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B84" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="C84" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="D84" s="80"/>
+      <c r="E84" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="F84" s="68"/>
+      <c r="G84" s="68"/>
+      <c r="H84" s="68" t="s">
         <v>144</v>
       </c>
-      <c r="C77" s="73"/>
-      <c r="D77" s="73"/>
-      <c r="E77" s="53"/>
-      <c r="F77" s="53"/>
-      <c r="G77" s="79" t="n">
-        <v>80</v>
-      </c>
-      <c r="H77" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="I77" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J77" s="79" t="n">
-        <v>80</v>
-      </c>
-      <c r="K77" s="73"/>
-      <c r="L77" s="73" t="s">
+      <c r="I84" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="J84" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="K84" s="77" t="n">
+        <v>1</v>
+      </c>
+      <c r="L84" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="M84" s="78" t="n">
+        <v>100.57</v>
+      </c>
+      <c r="N84" s="61" t="n">
+        <v>1005.7</v>
+      </c>
+      <c r="O84" s="61" t="n">
+        <v>16.83</v>
+      </c>
+      <c r="P84" s="61" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Q84" s="61" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="R84" s="61" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="S84" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="M77" s="53"/>
-      <c r="N77" s="53" t="n">
-        <v>60259</v>
-      </c>
-      <c r="O77" s="53" t="n">
-        <v>33</v>
-      </c>
-      <c r="P77" s="53"/>
-      <c r="Q77" s="53"/>
-      <c r="R77" s="53"/>
-      <c r="S77" s="53"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="11" t="s">
+      <c r="T84" s="61" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B85" s="72" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="D85" s="68"/>
+      <c r="E85" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="F85" s="68"/>
+      <c r="G85" s="68"/>
+      <c r="H85" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="I85" s="68" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="76" t="s">
-        <v>146</v>
-      </c>
-      <c r="C80" s="76"/>
-      <c r="D80" s="76"/>
-      <c r="E80" s="76"/>
-      <c r="F80" s="76"/>
-      <c r="G80" s="76"/>
-      <c r="H80" s="76"/>
-      <c r="I80" s="76"/>
-      <c r="J80" s="76"/>
-      <c r="K80" s="76"/>
-      <c r="L80" s="74"/>
-      <c r="M80" s="74"/>
-      <c r="N80" s="50"/>
-      <c r="O80" s="75"/>
-      <c r="P80" s="75"/>
-    </row>
-    <row r="81" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="70" t="s">
-        <v>147</v>
-      </c>
-      <c r="C81" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="D81" s="71"/>
-      <c r="E81" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="F81" s="71"/>
-      <c r="G81" s="71"/>
-      <c r="H81" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="I81" s="71" t="s">
-        <v>150</v>
-      </c>
-      <c r="J81" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="K81" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="L81" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="M81" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="N81" s="71" t="s">
-        <v>155</v>
-      </c>
-      <c r="O81" s="71" t="s">
-        <v>156</v>
-      </c>
-      <c r="P81" s="71" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q81" s="71" t="s">
-        <v>158</v>
-      </c>
-      <c r="R81" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="S81" s="71" t="s">
-        <v>160</v>
-      </c>
-      <c r="T81" s="71" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="72" t="s">
-        <v>162</v>
-      </c>
-      <c r="C82" s="80" t="s">
-        <v>163</v>
-      </c>
-      <c r="D82" s="80"/>
-      <c r="E82" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68" t="s">
-        <v>141</v>
-      </c>
-      <c r="I82" s="68" t="s">
-        <v>142</v>
-      </c>
-      <c r="J82" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="K82" s="77" t="n">
+      <c r="J85" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="K85" s="77" t="n">
         <v>1</v>
       </c>
-      <c r="L82" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="M82" s="78" t="n">
-        <v>100.57</v>
-      </c>
-      <c r="N82" s="61" t="n">
-        <v>1005.7</v>
-      </c>
-      <c r="O82" s="61" t="n">
-        <v>16.83</v>
-      </c>
-      <c r="P82" s="61" t="n">
+      <c r="L85" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="M85" s="78" t="n">
+        <v>100.41</v>
+      </c>
+      <c r="N85" s="61" t="n">
+        <v>1004.1</v>
+      </c>
+      <c r="O85" s="61" t="n">
+        <v>17.03</v>
+      </c>
+      <c r="P85" s="61" t="n">
         <v>0.04</v>
       </c>
-      <c r="Q82" s="61" t="n">
+      <c r="Q85" s="61" t="n">
         <v>0.04</v>
       </c>
-      <c r="R82" s="61" t="n">
+      <c r="R85" s="61" t="n">
         <v>0.02</v>
       </c>
-      <c r="S82" s="68" t="s">
+      <c r="S85" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="T82" s="61" t="n">
+      <c r="T85" s="61" t="n">
         <v>0.4</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="72" t="s">
-        <v>167</v>
-      </c>
-      <c r="C83" s="68" t="s">
-        <v>168</v>
-      </c>
-      <c r="D83" s="68"/>
-      <c r="E83" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68" t="s">
-        <v>141</v>
-      </c>
-      <c r="I83" s="68" t="s">
-        <v>142</v>
-      </c>
-      <c r="J83" s="68" t="s">
-        <v>169</v>
-      </c>
-      <c r="K83" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="L83" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="M83" s="78" t="n">
-        <v>100.41</v>
-      </c>
-      <c r="N83" s="61" t="n">
-        <v>1004.1</v>
-      </c>
-      <c r="O83" s="61" t="n">
-        <v>17.03</v>
-      </c>
-      <c r="P83" s="61" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="Q83" s="61" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="R83" s="61" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="S83" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="T83" s="61" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" s="73"/>
-      <c r="D84" s="73"/>
-      <c r="E84" s="73"/>
-      <c r="F84" s="73"/>
-      <c r="G84" s="73"/>
-      <c r="H84" s="73"/>
-      <c r="I84" s="73"/>
-      <c r="J84" s="73"/>
-      <c r="K84" s="79" t="n">
-        <v>2</v>
-      </c>
-      <c r="L84" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="M84" s="81"/>
-      <c r="N84" s="53" t="n">
-        <v>2009.8</v>
-      </c>
-      <c r="O84" s="53" t="n">
-        <v>33.86</v>
-      </c>
-      <c r="P84" s="53" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="Q84" s="53" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="R84" s="53" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="S84" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="T84" s="53" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="52" t="s">
-        <v>171</v>
-      </c>
-      <c r="C85" s="73"/>
-      <c r="D85" s="73"/>
-      <c r="E85" s="73"/>
-      <c r="F85" s="73"/>
-      <c r="G85" s="73"/>
-      <c r="H85" s="73"/>
-      <c r="I85" s="73"/>
-      <c r="J85" s="73"/>
-      <c r="K85" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="L85" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="M85" s="81"/>
-      <c r="N85" s="53" t="n">
-        <v>-1.6</v>
-      </c>
-      <c r="O85" s="53" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="P85" s="53" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="Q85" s="53" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="R85" s="53" t="n">
-        <v>-0.04</v>
-      </c>
-      <c r="S85" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="T85" s="53" t="n">
-        <v>-0.8</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="52" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C86" s="73"/>
       <c r="D86" s="73"/>
@@ -4615,303 +4628,301 @@
       <c r="I86" s="73"/>
       <c r="J86" s="73"/>
       <c r="K86" s="79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L86" s="73" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="M86" s="81"/>
       <c r="N86" s="53" t="n">
-        <v>1005.7</v>
+        <v>2009.8</v>
       </c>
       <c r="O86" s="53" t="n">
-        <v>16.83</v>
+        <v>33.86</v>
       </c>
       <c r="P86" s="53" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="Q86" s="53" t="n">
-        <v>-0.04</v>
+        <v>0.08</v>
       </c>
       <c r="R86" s="53" t="n">
-        <v>-0.02</v>
+        <v>0.02</v>
       </c>
       <c r="S86" s="73" t="s">
         <v>14</v>
       </c>
       <c r="T86" s="53" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B87" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="C87" s="73"/>
+      <c r="D87" s="73"/>
+      <c r="E87" s="73"/>
+      <c r="F87" s="73"/>
+      <c r="G87" s="73"/>
+      <c r="H87" s="73"/>
+      <c r="I87" s="73"/>
+      <c r="J87" s="73"/>
+      <c r="K87" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="M87" s="81"/>
+      <c r="N87" s="53" t="n">
+        <v>-1.6</v>
+      </c>
+      <c r="O87" s="53" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="P87" s="53" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="Q87" s="53" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="R87" s="53" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="S87" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="T87" s="53" t="n">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B88" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="C88" s="73"/>
+      <c r="D88" s="73"/>
+      <c r="E88" s="73"/>
+      <c r="F88" s="73"/>
+      <c r="G88" s="73"/>
+      <c r="H88" s="73"/>
+      <c r="I88" s="73"/>
+      <c r="J88" s="73"/>
+      <c r="K88" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L88" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="M88" s="81"/>
+      <c r="N88" s="53" t="n">
+        <v>1005.7</v>
+      </c>
+      <c r="O88" s="53" t="n">
+        <v>16.83</v>
+      </c>
+      <c r="P88" s="53" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Q88" s="53" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="R88" s="53" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="S88" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="T88" s="53" t="n">
         <v>0.4</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="82" t="s">
+    <row r="89" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B89" s="82" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="82"/>
+      <c r="D89" s="82"/>
+      <c r="E89" s="82"/>
+      <c r="F89" s="82"/>
+      <c r="G89" s="82"/>
+      <c r="H89" s="82"/>
+      <c r="I89" s="82"/>
+      <c r="J89" s="82"/>
+      <c r="K89" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="L89" s="82" t="s">
+        <v>169</v>
+      </c>
+      <c r="M89" s="84"/>
+      <c r="N89" s="85" t="n">
+        <v>1004.1</v>
+      </c>
+      <c r="O89" s="85" t="n">
+        <v>17.03</v>
+      </c>
+      <c r="P89" s="85" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Q89" s="85" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="R89" s="85" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="S89" s="82" t="s">
+        <v>14</v>
+      </c>
+      <c r="T89" s="85" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="C91" s="76"/>
+      <c r="D91" s="76"/>
+      <c r="E91" s="76"/>
+      <c r="F91" s="76"/>
+      <c r="G91" s="76"/>
+      <c r="H91" s="76"/>
+      <c r="I91" s="76"/>
+      <c r="J91" s="76"/>
+      <c r="K91" s="76"/>
+      <c r="L91" s="76"/>
+      <c r="M91" s="76"/>
+      <c r="N91" s="74"/>
+      <c r="O91" s="74"/>
+      <c r="P91" s="50"/>
+      <c r="Q91" s="75"/>
+      <c r="R91" s="75"/>
+    </row>
+    <row r="92" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B92" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="C92" s="71" t="s">
+        <v>179</v>
+      </c>
+      <c r="D92" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="E92" s="71"/>
+      <c r="F92" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="G92" s="71"/>
+      <c r="H92" s="71"/>
+      <c r="I92" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="J92" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="K92" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="L92" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="M92" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="N92" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="O92" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="P92" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q92" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="R92" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="S92" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="T92" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="U92" s="71" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B93" s="72" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="D93" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="E93" s="68"/>
+      <c r="F93" s="68" t="s">
+        <v>141</v>
+      </c>
+      <c r="G93" s="68"/>
+      <c r="H93" s="68"/>
+      <c r="I93" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="J93" s="68"/>
+      <c r="K93" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="L93" s="77" t="n">
+        <v>10</v>
+      </c>
+      <c r="M93" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="N93" s="78" t="n">
+        <v>987.65</v>
+      </c>
+      <c r="O93" s="61" t="n">
+        <v>9876.5</v>
+      </c>
+      <c r="P93" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="61" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R93" s="61" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S93" s="61" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="T93" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="U93" s="61" t="n">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="52" t="s">
         <v>173</v>
-      </c>
-      <c r="C87" s="82"/>
-      <c r="D87" s="82"/>
-      <c r="E87" s="82"/>
-      <c r="F87" s="82"/>
-      <c r="G87" s="82"/>
-      <c r="H87" s="82"/>
-      <c r="I87" s="82"/>
-      <c r="J87" s="82"/>
-      <c r="K87" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="L87" s="82" t="s">
-        <v>166</v>
-      </c>
-      <c r="M87" s="84"/>
-      <c r="N87" s="85" t="n">
-        <v>1004.1</v>
-      </c>
-      <c r="O87" s="85" t="n">
-        <v>17.03</v>
-      </c>
-      <c r="P87" s="85" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="Q87" s="85" t="n">
-        <v>-0.04</v>
-      </c>
-      <c r="R87" s="85" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="S87" s="82" t="s">
-        <v>14</v>
-      </c>
-      <c r="T87" s="85" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="C89" s="76"/>
-      <c r="D89" s="76"/>
-      <c r="E89" s="76"/>
-      <c r="F89" s="76"/>
-      <c r="G89" s="76"/>
-      <c r="H89" s="76"/>
-      <c r="I89" s="76"/>
-      <c r="J89" s="76"/>
-      <c r="K89" s="76"/>
-      <c r="L89" s="76"/>
-      <c r="M89" s="76"/>
-      <c r="N89" s="74"/>
-      <c r="O89" s="74"/>
-      <c r="P89" s="50"/>
-      <c r="Q89" s="75"/>
-      <c r="R89" s="75"/>
-    </row>
-    <row r="90" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="B90" s="70" t="s">
-        <v>147</v>
-      </c>
-      <c r="C90" s="71" t="s">
-        <v>176</v>
-      </c>
-      <c r="D90" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="E90" s="71"/>
-      <c r="F90" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="G90" s="71"/>
-      <c r="H90" s="71"/>
-      <c r="I90" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="J90" s="71" t="s">
-        <v>150</v>
-      </c>
-      <c r="K90" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="L90" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="M90" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="N90" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="O90" s="71" t="s">
-        <v>155</v>
-      </c>
-      <c r="P90" s="71" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q90" s="71" t="s">
-        <v>157</v>
-      </c>
-      <c r="R90" s="71" t="s">
-        <v>158</v>
-      </c>
-      <c r="S90" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="T90" s="71" t="s">
-        <v>160</v>
-      </c>
-      <c r="U90" s="71" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="B91" s="72" t="s">
-        <v>179</v>
-      </c>
-      <c r="C91" s="68" t="s">
-        <v>180</v>
-      </c>
-      <c r="D91" s="68" t="s">
-        <v>181</v>
-      </c>
-      <c r="E91" s="68"/>
-      <c r="F91" s="68" t="s">
-        <v>138</v>
-      </c>
-      <c r="G91" s="68"/>
-      <c r="H91" s="68"/>
-      <c r="I91" s="68" t="s">
-        <v>139</v>
-      </c>
-      <c r="J91" s="68"/>
-      <c r="K91" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="L91" s="77" t="n">
-        <v>10</v>
-      </c>
-      <c r="M91" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="N91" s="78" t="n">
-        <v>987.65</v>
-      </c>
-      <c r="O91" s="61" t="n">
-        <v>9876.5</v>
-      </c>
-      <c r="P91" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q91" s="61" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="R91" s="61" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="S91" s="61" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="T91" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="U91" s="61" t="n">
-        <v>5.67</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="B92" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="C92" s="73"/>
-      <c r="D92" s="73"/>
-      <c r="E92" s="73"/>
-      <c r="F92" s="73"/>
-      <c r="G92" s="73"/>
-      <c r="H92" s="73"/>
-      <c r="I92" s="73"/>
-      <c r="J92" s="73"/>
-      <c r="K92" s="73"/>
-      <c r="L92" s="79" t="n">
-        <v>10</v>
-      </c>
-      <c r="M92" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="N92" s="81"/>
-      <c r="O92" s="53" t="n">
-        <v>9876.5</v>
-      </c>
-      <c r="P92" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q92" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="R92" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="S92" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="T92" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="U92" s="53" t="n">
-        <v>5.67</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="52" t="s">
-        <v>171</v>
-      </c>
-      <c r="C93" s="73"/>
-      <c r="D93" s="73"/>
-      <c r="E93" s="73"/>
-      <c r="F93" s="73"/>
-      <c r="G93" s="73"/>
-      <c r="H93" s="73"/>
-      <c r="I93" s="73"/>
-      <c r="J93" s="73"/>
-      <c r="K93" s="73"/>
-      <c r="L93" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="M93" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="N93" s="81"/>
-      <c r="O93" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="P93" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q93" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="R93" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="S93" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="T93" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="U93" s="53" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="52" t="s">
-        <v>172</v>
       </c>
       <c r="C94" s="73"/>
       <c r="D94" s="73"/>
@@ -4926,7 +4937,7 @@
         <v>10</v>
       </c>
       <c r="M94" s="73" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N94" s="81"/>
       <c r="O94" s="53" t="n">
@@ -4951,277 +4962,277 @@
         <v>5.67</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="82" t="s">
-        <v>173</v>
-      </c>
-      <c r="C95" s="82"/>
-      <c r="D95" s="82"/>
-      <c r="E95" s="82"/>
-      <c r="F95" s="82"/>
-      <c r="G95" s="82"/>
-      <c r="H95" s="82"/>
-      <c r="I95" s="82"/>
-      <c r="J95" s="82"/>
-      <c r="K95" s="82"/>
-      <c r="L95" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="M95" s="82" t="s">
-        <v>166</v>
-      </c>
-      <c r="N95" s="84"/>
-      <c r="O95" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="P95" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q95" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="R95" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="S95" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="T95" s="82" t="s">
+    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="C95" s="73"/>
+      <c r="D95" s="73"/>
+      <c r="E95" s="73"/>
+      <c r="F95" s="73"/>
+      <c r="G95" s="73"/>
+      <c r="H95" s="73"/>
+      <c r="I95" s="73"/>
+      <c r="J95" s="73"/>
+      <c r="K95" s="73"/>
+      <c r="L95" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="N95" s="81"/>
+      <c r="O95" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="P95" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="R95" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="T95" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="U95" s="85" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="76" t="s">
-        <v>184</v>
-      </c>
-      <c r="C97" s="76"/>
-      <c r="D97" s="76"/>
-      <c r="E97" s="76"/>
-      <c r="F97" s="76"/>
-      <c r="G97" s="76"/>
-      <c r="H97" s="76"/>
-      <c r="I97" s="76"/>
-      <c r="J97" s="76"/>
-      <c r="K97" s="76"/>
-      <c r="L97" s="76"/>
-      <c r="M97" s="76"/>
-      <c r="N97" s="74"/>
-      <c r="O97" s="74"/>
-      <c r="P97" s="50"/>
-      <c r="Q97" s="75"/>
-      <c r="R97" s="75"/>
-    </row>
-    <row r="98" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="U95" s="53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="C96" s="73"/>
+      <c r="D96" s="73"/>
+      <c r="E96" s="73"/>
+      <c r="F96" s="73"/>
+      <c r="G96" s="73"/>
+      <c r="H96" s="73"/>
+      <c r="I96" s="73"/>
+      <c r="J96" s="73"/>
+      <c r="K96" s="73"/>
+      <c r="L96" s="79" t="n">
+        <v>10</v>
+      </c>
+      <c r="M96" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="N96" s="81"/>
+      <c r="O96" s="53" t="n">
+        <v>9876.5</v>
+      </c>
+      <c r="P96" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="R96" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="S96" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="T96" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="U96" s="53" t="n">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="82" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" s="82"/>
+      <c r="D97" s="82"/>
+      <c r="E97" s="82"/>
+      <c r="F97" s="82"/>
+      <c r="G97" s="82"/>
+      <c r="H97" s="82"/>
+      <c r="I97" s="82"/>
+      <c r="J97" s="82"/>
+      <c r="K97" s="82"/>
+      <c r="L97" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" s="82" t="s">
+        <v>169</v>
+      </c>
+      <c r="N97" s="84"/>
+      <c r="O97" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P97" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="R97" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="S97" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T97" s="82" t="s">
+        <v>14</v>
+      </c>
+      <c r="U97" s="85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="B98" s="70" t="s">
-        <v>147</v>
-      </c>
-      <c r="C98" s="71" t="s">
         <v>186</v>
       </c>
-      <c r="D98" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="E98" s="71"/>
-      <c r="F98" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="G98" s="71"/>
-      <c r="H98" s="71"/>
-      <c r="I98" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="J98" s="71" t="s">
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="C99" s="76"/>
+      <c r="D99" s="76"/>
+      <c r="E99" s="76"/>
+      <c r="F99" s="76"/>
+      <c r="G99" s="76"/>
+      <c r="H99" s="76"/>
+      <c r="I99" s="76"/>
+      <c r="J99" s="76"/>
+      <c r="K99" s="76"/>
+      <c r="L99" s="76"/>
+      <c r="M99" s="76"/>
+      <c r="N99" s="74"/>
+      <c r="O99" s="74"/>
+      <c r="P99" s="50"/>
+      <c r="Q99" s="75"/>
+      <c r="R99" s="75"/>
+    </row>
+    <row r="100" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B100" s="70" t="s">
         <v>150</v>
       </c>
-      <c r="K98" s="71" t="s">
+      <c r="C100" s="71" t="s">
+        <v>189</v>
+      </c>
+      <c r="D100" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="L98" s="71" t="s">
+      <c r="E100" s="71"/>
+      <c r="F100" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="M98" s="71" t="s">
+      <c r="G100" s="71"/>
+      <c r="H100" s="71"/>
+      <c r="I100" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="J100" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="N98" s="71" t="s">
+      <c r="K100" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="O98" s="71" t="s">
+      <c r="L100" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="P98" s="71" t="s">
+      <c r="M100" s="71" t="s">
         <v>156</v>
       </c>
-      <c r="Q98" s="71" t="s">
+      <c r="N100" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="R98" s="71" t="s">
+      <c r="O100" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="S98" s="71" t="s">
+      <c r="P100" s="71" t="s">
         <v>159</v>
       </c>
-      <c r="T98" s="71" t="s">
+      <c r="Q100" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="U98" s="71" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="B99" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="C99" s="68" t="s">
-        <v>189</v>
-      </c>
-      <c r="D99" s="68" t="s">
+      <c r="R100" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="S100" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="T100" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="U100" s="71" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="E99" s="68"/>
-      <c r="F99" s="68" t="s">
+      <c r="B101" s="72" t="s">
         <v>191</v>
       </c>
-      <c r="G99" s="68"/>
-      <c r="H99" s="68"/>
-      <c r="I99" s="68" t="s">
+      <c r="C101" s="68" t="s">
         <v>192</v>
       </c>
-      <c r="J99" s="68"/>
-      <c r="K99" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="L99" s="77" t="n">
+      <c r="D101" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="E101" s="68"/>
+      <c r="F101" s="68" t="s">
+        <v>194</v>
+      </c>
+      <c r="G101" s="68"/>
+      <c r="H101" s="68"/>
+      <c r="I101" s="68" t="s">
+        <v>195</v>
+      </c>
+      <c r="J101" s="68"/>
+      <c r="K101" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="L101" s="77" t="n">
         <v>10</v>
       </c>
-      <c r="M99" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="N99" s="78" t="n">
+      <c r="M101" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="N101" s="78" t="n">
         <v>1532.1</v>
       </c>
-      <c r="O99" s="61" t="n">
+      <c r="O101" s="61" t="n">
         <v>15321</v>
       </c>
-      <c r="P99" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q99" s="61" t="n">
+      <c r="P101" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="61" t="n">
         <v>0.6</v>
       </c>
-      <c r="R99" s="61" t="n">
+      <c r="R101" s="61" t="n">
         <v>0.5</v>
       </c>
-      <c r="S99" s="61" t="n">
+      <c r="S101" s="61" t="n">
         <v>0.45</v>
       </c>
-      <c r="T99" s="68" t="s">
+      <c r="T101" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="U99" s="61" t="n">
+      <c r="U101" s="61" t="n">
         <v>7.11</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="C100" s="73"/>
-      <c r="D100" s="73"/>
-      <c r="E100" s="73"/>
-      <c r="F100" s="73"/>
-      <c r="G100" s="73"/>
-      <c r="H100" s="73"/>
-      <c r="I100" s="73"/>
-      <c r="J100" s="73"/>
-      <c r="K100" s="73"/>
-      <c r="L100" s="79" t="n">
-        <v>10</v>
-      </c>
-      <c r="M100" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="N100" s="81"/>
-      <c r="O100" s="53" t="n">
-        <v>15321</v>
-      </c>
-      <c r="P100" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q100" s="53" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="R100" s="53" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="S100" s="53" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="T100" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="U100" s="53" t="n">
-        <v>7.11</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="52" t="s">
-        <v>171</v>
-      </c>
-      <c r="C101" s="73"/>
-      <c r="D101" s="73"/>
-      <c r="E101" s="73"/>
-      <c r="F101" s="73"/>
-      <c r="G101" s="73"/>
-      <c r="H101" s="73"/>
-      <c r="I101" s="73"/>
-      <c r="J101" s="73"/>
-      <c r="K101" s="73"/>
-      <c r="L101" s="79" t="n">
-        <v>10</v>
-      </c>
-      <c r="M101" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="N101" s="81"/>
-      <c r="O101" s="53" t="n">
-        <v>-15321</v>
-      </c>
-      <c r="P101" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q101" s="53" t="n">
-        <v>-0.6</v>
-      </c>
-      <c r="R101" s="53" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="S101" s="53" t="n">
-        <v>-0.45</v>
-      </c>
-      <c r="T101" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="U101" s="53" t="n">
-        <v>-7.11</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="52" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C102" s="73"/>
       <c r="D102" s="73"/>
@@ -5236,7 +5247,7 @@
         <v>10</v>
       </c>
       <c r="M102" s="73" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N102" s="81"/>
       <c r="O102" s="53" t="n">
@@ -5262,545 +5273,737 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="82" t="s">
-        <v>173</v>
-      </c>
-      <c r="C103" s="82"/>
-      <c r="D103" s="82"/>
-      <c r="E103" s="82"/>
-      <c r="F103" s="82"/>
-      <c r="G103" s="82"/>
-      <c r="H103" s="82"/>
-      <c r="I103" s="82"/>
-      <c r="J103" s="82"/>
-      <c r="K103" s="82"/>
-      <c r="L103" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="M103" s="82" t="s">
-        <v>166</v>
-      </c>
-      <c r="N103" s="84"/>
-      <c r="O103" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="P103" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q103" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="R103" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="S103" s="85" t="n">
-        <v>0</v>
-      </c>
-      <c r="T103" s="82" t="s">
+      <c r="B103" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="C103" s="73"/>
+      <c r="D103" s="73"/>
+      <c r="E103" s="73"/>
+      <c r="F103" s="73"/>
+      <c r="G103" s="73"/>
+      <c r="H103" s="73"/>
+      <c r="I103" s="73"/>
+      <c r="J103" s="73"/>
+      <c r="K103" s="73"/>
+      <c r="L103" s="79" t="n">
+        <v>10</v>
+      </c>
+      <c r="M103" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="N103" s="81"/>
+      <c r="O103" s="53" t="n">
+        <v>-15321</v>
+      </c>
+      <c r="P103" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="53" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="R103" s="53" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="S103" s="53" t="n">
+        <v>-0.45</v>
+      </c>
+      <c r="T103" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="U103" s="85" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="23"/>
-    </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="76" t="s">
-        <v>193</v>
-      </c>
-      <c r="C105" s="76"/>
-      <c r="D105" s="76"/>
-      <c r="E105" s="76"/>
-      <c r="F105" s="76"/>
-      <c r="G105" s="76"/>
-      <c r="H105" s="74"/>
-      <c r="I105" s="74"/>
-      <c r="J105" s="50"/>
-      <c r="K105" s="75"/>
-      <c r="L105" s="75"/>
-    </row>
-    <row r="106" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="B106" s="86" t="s">
-        <v>195</v>
-      </c>
-      <c r="C106" s="71" t="s">
+      <c r="U103" s="53" t="n">
+        <v>-7.11</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="C104" s="73"/>
+      <c r="D104" s="73"/>
+      <c r="E104" s="73"/>
+      <c r="F104" s="73"/>
+      <c r="G104" s="73"/>
+      <c r="H104" s="73"/>
+      <c r="I104" s="73"/>
+      <c r="J104" s="73"/>
+      <c r="K104" s="73"/>
+      <c r="L104" s="79" t="n">
+        <v>10</v>
+      </c>
+      <c r="M104" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="N104" s="81"/>
+      <c r="O104" s="53" t="n">
+        <v>15321</v>
+      </c>
+      <c r="P104" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" s="53" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="R104" s="53" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S104" s="53" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="T104" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="U104" s="53" t="n">
+        <v>7.11</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="82" t="s">
+        <v>176</v>
+      </c>
+      <c r="C105" s="82"/>
+      <c r="D105" s="82"/>
+      <c r="E105" s="82"/>
+      <c r="F105" s="82"/>
+      <c r="G105" s="82"/>
+      <c r="H105" s="82"/>
+      <c r="I105" s="82"/>
+      <c r="J105" s="82"/>
+      <c r="K105" s="82"/>
+      <c r="L105" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" s="82" t="s">
+        <v>169</v>
+      </c>
+      <c r="N105" s="84"/>
+      <c r="O105" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P105" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="R105" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="S105" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T105" s="82" t="s">
+        <v>14</v>
+      </c>
+      <c r="U105" s="85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="23"/>
+    </row>
+    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="D106" s="71"/>
-      <c r="E106" s="71"/>
-      <c r="F106" s="71"/>
-      <c r="G106" s="71"/>
-      <c r="H106" s="71" t="s">
+      <c r="C107" s="76"/>
+      <c r="D107" s="76"/>
+      <c r="E107" s="76"/>
+      <c r="F107" s="76"/>
+      <c r="G107" s="76"/>
+      <c r="H107" s="74"/>
+      <c r="I107" s="74"/>
+      <c r="J107" s="50"/>
+      <c r="K107" s="75"/>
+      <c r="L107" s="75"/>
+    </row>
+    <row r="108" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="I106" s="71" t="s">
+      <c r="B108" s="86" t="s">
         <v>198</v>
       </c>
-      <c r="J106" s="71" t="s">
+      <c r="C108" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="K106" s="71" t="s">
+      <c r="D108" s="71"/>
+      <c r="E108" s="71"/>
+      <c r="F108" s="71"/>
+      <c r="G108" s="71"/>
+      <c r="H108" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="L106" s="71" t="s">
+      <c r="I108" s="71" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="107" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="86"/>
-      <c r="C107" s="86"/>
-      <c r="D107" s="86"/>
-      <c r="E107" s="86"/>
-      <c r="F107" s="86"/>
-      <c r="G107" s="86"/>
-      <c r="H107" s="86" t="s">
+      <c r="J108" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="I107" s="86" t="s">
+      <c r="K108" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="J107" s="86" t="s">
+      <c r="L108" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="K107" s="86" t="s">
+    </row>
+    <row r="109" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="86"/>
+      <c r="C109" s="86"/>
+      <c r="D109" s="86"/>
+      <c r="E109" s="86"/>
+      <c r="F109" s="86"/>
+      <c r="G109" s="86"/>
+      <c r="H109" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="L107" s="86" t="s">
+      <c r="I109" s="86" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="23" t="s">
+      <c r="J109" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="B108" s="72" t="s">
+      <c r="K109" s="86" t="s">
+        <v>208</v>
+      </c>
+      <c r="L109" s="86" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A110" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B110" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C108" s="68" t="s">
+      <c r="C110" s="68" t="s">
+        <v>211</v>
+      </c>
+      <c r="D110" s="68"/>
+      <c r="E110" s="68"/>
+      <c r="F110" s="68"/>
+      <c r="G110" s="68"/>
+      <c r="H110" s="61" t="n">
+        <v>18298.06</v>
+      </c>
+      <c r="I110" s="61" t="n">
+        <v>310.85</v>
+      </c>
+      <c r="J110" s="61" t="n">
+        <v>18585.98</v>
+      </c>
+      <c r="K110" s="61" t="n">
+        <v>18585.98</v>
+      </c>
+      <c r="L110" s="61" t="n">
+        <v>18585.98</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A111" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="B111" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="D111" s="68"/>
+      <c r="E111" s="68"/>
+      <c r="F111" s="68"/>
+      <c r="G111" s="68"/>
+      <c r="H111" s="61" t="n">
+        <v>-17987.21</v>
+      </c>
+      <c r="I111" s="61" t="n">
+        <v>18275.13</v>
+      </c>
+      <c r="J111" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L111" s="61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="B112" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112" s="87" t="s">
+        <v>215</v>
+      </c>
+      <c r="D112" s="87"/>
+      <c r="E112" s="87"/>
+      <c r="F112" s="87"/>
+      <c r="G112" s="87"/>
+      <c r="H112" s="88" t="n">
+        <v>310.85</v>
+      </c>
+      <c r="I112" s="88" t="n">
+        <v>18585.98</v>
+      </c>
+      <c r="J112" s="88" t="n">
+        <v>18585.98</v>
+      </c>
+      <c r="K112" s="88" t="n">
+        <v>18585.98</v>
+      </c>
+      <c r="L112" s="88" t="n">
+        <v>18585.98</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="76" t="s">
+        <v>217</v>
+      </c>
+      <c r="C114" s="76"/>
+      <c r="D114" s="76"/>
+      <c r="E114" s="76"/>
+      <c r="F114" s="76"/>
+      <c r="G114" s="76"/>
+      <c r="H114" s="74"/>
+      <c r="I114" s="74"/>
+      <c r="J114" s="50"/>
+      <c r="K114" s="75"/>
+      <c r="L114" s="75"/>
+    </row>
+    <row r="115" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B115" s="86" t="s">
+        <v>219</v>
+      </c>
+      <c r="C115" s="86"/>
+      <c r="D115" s="86"/>
+      <c r="E115" s="86" t="s">
+        <v>199</v>
+      </c>
+      <c r="F115" s="86"/>
+      <c r="G115" s="86"/>
+      <c r="H115" s="86"/>
+      <c r="I115" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="J115" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="K115" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="L115" s="71" t="s">
+        <v>203</v>
+      </c>
+      <c r="M115" s="71" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="34.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="86"/>
+      <c r="C116" s="86"/>
+      <c r="D116" s="86"/>
+      <c r="E116" s="86"/>
+      <c r="F116" s="86"/>
+      <c r="G116" s="86"/>
+      <c r="H116" s="86"/>
+      <c r="I116" s="86" t="s">
+        <v>205</v>
+      </c>
+      <c r="J116" s="86" t="s">
+        <v>206</v>
+      </c>
+      <c r="K116" s="86" t="s">
+        <v>207</v>
+      </c>
+      <c r="L116" s="86" t="s">
         <v>208</v>
       </c>
-      <c r="D108" s="68"/>
-      <c r="E108" s="68"/>
-      <c r="F108" s="68"/>
-      <c r="G108" s="68"/>
-      <c r="H108" s="61" t="n">
-        <v>18298.06</v>
-      </c>
-      <c r="I108" s="61" t="n">
-        <v>310.85</v>
-      </c>
-      <c r="J108" s="61" t="n">
-        <v>18585.98</v>
-      </c>
-      <c r="K108" s="61" t="n">
-        <v>18585.98</v>
-      </c>
-      <c r="L108" s="61" t="n">
-        <v>18585.98</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="23" t="s">
+      <c r="M116" s="86" t="s">
         <v>209</v>
-      </c>
-      <c r="B109" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="C109" s="68" t="s">
-        <v>210</v>
-      </c>
-      <c r="D109" s="68"/>
-      <c r="E109" s="68"/>
-      <c r="F109" s="68"/>
-      <c r="G109" s="68"/>
-      <c r="H109" s="61" t="n">
-        <v>-17987.21</v>
-      </c>
-      <c r="I109" s="61" t="n">
-        <v>18275.13</v>
-      </c>
-      <c r="J109" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="K109" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L109" s="61" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="B110" s="87" t="s">
-        <v>14</v>
-      </c>
-      <c r="C110" s="87" t="s">
-        <v>212</v>
-      </c>
-      <c r="D110" s="87"/>
-      <c r="E110" s="87"/>
-      <c r="F110" s="87"/>
-      <c r="G110" s="87"/>
-      <c r="H110" s="88" t="n">
-        <v>310.85</v>
-      </c>
-      <c r="I110" s="88" t="n">
-        <v>18585.98</v>
-      </c>
-      <c r="J110" s="88" t="n">
-        <v>18585.98</v>
-      </c>
-      <c r="K110" s="88" t="n">
-        <v>18585.98</v>
-      </c>
-      <c r="L110" s="88" t="n">
-        <v>18585.98</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="23" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="76" t="s">
-        <v>214</v>
-      </c>
-      <c r="C112" s="76"/>
-      <c r="D112" s="76"/>
-      <c r="E112" s="76"/>
-      <c r="F112" s="76"/>
-      <c r="G112" s="76"/>
-      <c r="H112" s="74"/>
-      <c r="I112" s="74"/>
-      <c r="J112" s="50"/>
-      <c r="K112" s="75"/>
-      <c r="L112" s="75"/>
-    </row>
-    <row r="113" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="B113" s="86" t="s">
-        <v>216</v>
-      </c>
-      <c r="C113" s="86"/>
-      <c r="D113" s="86"/>
-      <c r="E113" s="86" t="s">
-        <v>196</v>
-      </c>
-      <c r="F113" s="86"/>
-      <c r="G113" s="86"/>
-      <c r="H113" s="86"/>
-      <c r="I113" s="71" t="s">
-        <v>197</v>
-      </c>
-      <c r="J113" s="71" t="s">
-        <v>198</v>
-      </c>
-      <c r="K113" s="71" t="s">
-        <v>199</v>
-      </c>
-      <c r="L113" s="71" t="s">
-        <v>200</v>
-      </c>
-      <c r="M113" s="71" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="34.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="86"/>
-      <c r="C114" s="86"/>
-      <c r="D114" s="86"/>
-      <c r="E114" s="86"/>
-      <c r="F114" s="86"/>
-      <c r="G114" s="86"/>
-      <c r="H114" s="86"/>
-      <c r="I114" s="86" t="s">
-        <v>202</v>
-      </c>
-      <c r="J114" s="86" t="s">
-        <v>203</v>
-      </c>
-      <c r="K114" s="86" t="s">
-        <v>204</v>
-      </c>
-      <c r="L114" s="86" t="s">
-        <v>205</v>
-      </c>
-      <c r="M114" s="86" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="B115" s="72" t="s">
-        <v>218</v>
-      </c>
-      <c r="C115" s="72"/>
-      <c r="D115" s="72"/>
-      <c r="E115" s="68" t="s">
-        <v>208</v>
-      </c>
-      <c r="F115" s="68"/>
-      <c r="G115" s="68"/>
-      <c r="H115" s="68"/>
-      <c r="I115" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="J115" s="77" t="n">
-        <v>3</v>
-      </c>
-      <c r="K115" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="L115" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="M115" s="77" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="B116" s="72" t="s">
-        <v>218</v>
-      </c>
-      <c r="C116" s="72"/>
-      <c r="D116" s="72"/>
-      <c r="E116" s="68" t="s">
-        <v>210</v>
-      </c>
-      <c r="F116" s="68"/>
-      <c r="G116" s="68"/>
-      <c r="H116" s="68"/>
-      <c r="I116" s="77" t="n">
-        <v>3</v>
-      </c>
-      <c r="J116" s="77" t="n">
-        <v>-3</v>
-      </c>
-      <c r="K116" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="L116" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="M116" s="77" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="B117" s="87" t="s">
-        <v>218</v>
-      </c>
-      <c r="C117" s="87"/>
-      <c r="D117" s="87"/>
-      <c r="E117" s="87" t="s">
-        <v>212</v>
-      </c>
-      <c r="F117" s="87"/>
-      <c r="G117" s="87"/>
-      <c r="H117" s="87"/>
-      <c r="I117" s="83" t="n">
+      <c r="B117" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="C117" s="72"/>
+      <c r="D117" s="72"/>
+      <c r="E117" s="68" t="s">
+        <v>211</v>
+      </c>
+      <c r="F117" s="68"/>
+      <c r="G117" s="68"/>
+      <c r="H117" s="68"/>
+      <c r="I117" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J117" s="77" t="n">
         <v>3</v>
       </c>
-      <c r="J117" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="K117" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="L117" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="M117" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K117" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M117" s="77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B118" s="72" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="76" t="s">
-        <v>222</v>
-      </c>
-      <c r="C119" s="76"/>
-      <c r="D119" s="74"/>
-      <c r="E119" s="74"/>
-      <c r="F119" s="50"/>
-      <c r="G119" s="75"/>
-      <c r="H119" s="75"/>
-    </row>
-    <row r="120" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="71" t="s">
+      <c r="C118" s="72"/>
+      <c r="D118" s="72"/>
+      <c r="E118" s="68" t="s">
+        <v>213</v>
+      </c>
+      <c r="F118" s="68"/>
+      <c r="G118" s="68"/>
+      <c r="H118" s="68"/>
+      <c r="I118" s="77" t="n">
+        <v>3</v>
+      </c>
+      <c r="J118" s="77" t="n">
+        <v>-3</v>
+      </c>
+      <c r="K118" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="L118" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" s="77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A119" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="C120" s="71" t="s">
-        <v>122</v>
-      </c>
-      <c r="D120" s="71"/>
-      <c r="E120" s="71"/>
-      <c r="F120" s="71"/>
-      <c r="G120" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="H120" s="71" t="s">
-        <v>150</v>
-      </c>
-      <c r="I120" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="J120" s="71" t="s">
-        <v>127</v>
-      </c>
-      <c r="K120" s="71" t="s">
+      <c r="B119" s="87" t="s">
+        <v>221</v>
+      </c>
+      <c r="C119" s="87"/>
+      <c r="D119" s="87"/>
+      <c r="E119" s="87" t="s">
+        <v>215</v>
+      </c>
+      <c r="F119" s="87"/>
+      <c r="G119" s="87"/>
+      <c r="H119" s="87"/>
+      <c r="I119" s="83" t="n">
+        <v>3</v>
+      </c>
+      <c r="J119" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="L119" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" s="83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="L120" s="71" t="s">
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="76" t="s">
         <v>225</v>
       </c>
-      <c r="M120" s="71" t="s">
+      <c r="C121" s="76"/>
+      <c r="D121" s="76"/>
+      <c r="E121" s="89"/>
+      <c r="F121" s="89"/>
+      <c r="G121" s="90"/>
+      <c r="H121" s="75"/>
+      <c r="I121" s="75"/>
+    </row>
+    <row r="122" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B122" s="71" t="s">
         <v>226</v>
       </c>
-      <c r="N120" s="71" t="s">
+      <c r="C122" s="71" t="s">
         <v>227</v>
       </c>
-      <c r="O120" s="71" t="s">
+      <c r="D122" s="71"/>
+      <c r="E122" s="71" t="s">
+        <v>125</v>
+      </c>
+      <c r="F122" s="71"/>
+      <c r="G122" s="71"/>
+      <c r="H122" s="71"/>
+      <c r="I122" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="J122" s="71" t="s">
         <v>228</v>
       </c>
-      <c r="P120" s="71" t="s">
+      <c r="K122" s="71" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="121" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="72" t="s">
+      <c r="L122" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="M122" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="N122" s="71" t="s">
         <v>230</v>
       </c>
-      <c r="C121" s="68" t="s">
+      <c r="O122" s="71" t="s">
         <v>231</v>
       </c>
-      <c r="D121" s="68"/>
-      <c r="E121" s="68"/>
-      <c r="F121" s="68"/>
-      <c r="G121" s="68" t="s">
+      <c r="P122" s="71" t="s">
         <v>232</v>
       </c>
-      <c r="H121" s="68" t="s">
+      <c r="Q122" s="71" t="s">
         <v>233</v>
       </c>
-      <c r="I121" s="77" t="n">
+      <c r="R122" s="71" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B123" s="72" t="s">
+        <v>235</v>
+      </c>
+      <c r="C123" s="68" t="s">
+        <v>236</v>
+      </c>
+      <c r="D123" s="68"/>
+      <c r="E123" s="68" t="s">
+        <v>237</v>
+      </c>
+      <c r="F123" s="68"/>
+      <c r="G123" s="68"/>
+      <c r="H123" s="68"/>
+      <c r="I123" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="J123" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="K123" s="77" t="n">
+        <v>8</v>
+      </c>
+      <c r="L123" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="M123" s="61" t="n">
+        <v>455.12</v>
+      </c>
+      <c r="N123" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P123" s="61" t="n">
+        <v>455.12</v>
+      </c>
+      <c r="Q123" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="R123" s="68" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="23"/>
+    </row>
+    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="76" t="s">
+        <v>240</v>
+      </c>
+      <c r="C126" s="76"/>
+      <c r="D126" s="74"/>
+      <c r="E126" s="74"/>
+      <c r="F126" s="50"/>
+      <c r="G126" s="75"/>
+      <c r="H126" s="75"/>
+    </row>
+    <row r="127" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B127" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="C127" s="71" t="s">
+        <v>125</v>
+      </c>
+      <c r="D127" s="71"/>
+      <c r="E127" s="71"/>
+      <c r="F127" s="71"/>
+      <c r="G127" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="H127" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="I127" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="J127" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="K127" s="71" t="s">
+        <v>241</v>
+      </c>
+      <c r="L127" s="71" t="s">
+        <v>242</v>
+      </c>
+      <c r="M127" s="71" t="s">
+        <v>243</v>
+      </c>
+      <c r="N127" s="71" t="s">
+        <v>244</v>
+      </c>
+      <c r="O127" s="71" t="s">
+        <v>232</v>
+      </c>
+      <c r="P127" s="71" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B128" s="72" t="s">
+        <v>245</v>
+      </c>
+      <c r="C128" s="68" t="s">
+        <v>246</v>
+      </c>
+      <c r="D128" s="68"/>
+      <c r="E128" s="68"/>
+      <c r="F128" s="68"/>
+      <c r="G128" s="68" t="s">
+        <v>247</v>
+      </c>
+      <c r="H128" s="68" t="s">
+        <v>248</v>
+      </c>
+      <c r="I128" s="77" t="n">
         <v>10</v>
       </c>
-      <c r="J121" s="68" t="s">
+      <c r="J128" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="K121" s="78" t="n">
+      <c r="K128" s="78" t="n">
         <v>141.75</v>
       </c>
-      <c r="L121" s="61" t="n">
+      <c r="L128" s="61" t="n">
         <v>1417.5</v>
       </c>
-      <c r="M121" s="61" t="n">
+      <c r="M128" s="61" t="n">
         <v>184</v>
       </c>
-      <c r="N121" s="61" t="s">
+      <c r="N128" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="O121" s="61" t="n">
+      <c r="O128" s="61" t="n">
         <v>1233.5</v>
       </c>
-      <c r="P121" s="68" t="s">
+      <c r="P128" s="68" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="34"/>
-      <c r="B130" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C130" s="34"/>
-      <c r="D130" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="34"/>
-      <c r="B132" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="C132" s="38"/>
-      <c r="D132" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="E132" s="11"/>
-      <c r="F132" s="34"/>
-      <c r="G132" s="34"/>
-      <c r="H132" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="I132" s="34"/>
-      <c r="J132" s="34"/>
-      <c r="K132" s="34"/>
-      <c r="L132" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="M132" s="34"/>
-      <c r="N132" s="34"/>
-    </row>
-    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="B133" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="C133" s="23" t="n">
+    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A137" s="34"/>
+      <c r="B137" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C137" s="34"/>
+      <c r="D137" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A139" s="34"/>
+      <c r="B139" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C139" s="38"/>
+      <c r="D139" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="E139" s="11"/>
+      <c r="F139" s="34"/>
+      <c r="G139" s="34"/>
+      <c r="H139" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="I139" s="34"/>
+      <c r="J139" s="34"/>
+      <c r="K139" s="34"/>
+      <c r="L139" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="M139" s="34"/>
+      <c r="N139" s="34"/>
+    </row>
+    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A140" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="B140" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="C140" s="23" t="n">
         <v>82</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="B135" s="89" t="s">
-        <v>242</v>
-      </c>
-      <c r="C135" s="89"/>
-      <c r="D135" s="89"/>
-      <c r="E135" s="89"/>
-      <c r="F135" s="89"/>
-      <c r="G135" s="89"/>
-      <c r="H135" s="89"/>
-      <c r="I135" s="89"/>
-      <c r="J135" s="89"/>
-      <c r="K135" s="89"/>
-      <c r="L135" s="89"/>
-      <c r="M135" s="89"/>
-      <c r="N135" s="89"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A142" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B142" s="91" t="s">
+        <v>257</v>
+      </c>
+      <c r="C142" s="91"/>
+      <c r="D142" s="91"/>
+      <c r="E142" s="91"/>
+      <c r="F142" s="91"/>
+      <c r="G142" s="91"/>
+      <c r="H142" s="91"/>
+      <c r="I142" s="91"/>
+      <c r="J142" s="91"/>
+      <c r="K142" s="91"/>
+      <c r="L142" s="91"/>
+      <c r="M142" s="91"/>
+      <c r="N142" s="91"/>
+    </row>
   </sheetData>
-  <mergeCells count="129">
+  <mergeCells count="140">
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B9:C9"/>
@@ -5863,17 +6066,19 @@
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="F70:G70"/>
     <mergeCell ref="H70:L70"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:L71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="H72:L72"/>
+    <mergeCell ref="B74:E74"/>
     <mergeCell ref="B75:D75"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B80:K80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B82:K82"/>
     <mergeCell ref="C83:D83"/>
     <mergeCell ref="E83:G83"/>
     <mergeCell ref="C84:D84"/>
@@ -5884,11 +6089,11 @@
     <mergeCell ref="E86:G86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="E87:G87"/>
-    <mergeCell ref="B89:M89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="B91:M91"/>
     <mergeCell ref="D92:E92"/>
     <mergeCell ref="F92:H92"/>
     <mergeCell ref="D93:E93"/>
@@ -5897,11 +6102,11 @@
     <mergeCell ref="F94:H94"/>
     <mergeCell ref="D95:E95"/>
     <mergeCell ref="F95:H95"/>
-    <mergeCell ref="B97:M97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="B99:M99"/>
     <mergeCell ref="D100:E100"/>
     <mergeCell ref="F100:H100"/>
     <mergeCell ref="D101:E101"/>
@@ -5910,26 +6115,35 @@
     <mergeCell ref="F102:H102"/>
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="F103:H103"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="B107:G107"/>
+    <mergeCell ref="B108:B109"/>
     <mergeCell ref="C108:G108"/>
     <mergeCell ref="C109:G109"/>
     <mergeCell ref="C110:G110"/>
-    <mergeCell ref="B112:G112"/>
-    <mergeCell ref="B113:D114"/>
-    <mergeCell ref="E113:H114"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="E115:H115"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="E116:H116"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="B114:G114"/>
+    <mergeCell ref="B115:D116"/>
+    <mergeCell ref="E115:H116"/>
     <mergeCell ref="B117:D117"/>
     <mergeCell ref="E117:H117"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="C120:F120"/>
-    <mergeCell ref="C121:F121"/>
-    <mergeCell ref="B135:N135"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="E118:H118"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="E119:H119"/>
+    <mergeCell ref="B121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="E122:H122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="E123:H123"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="C127:F127"/>
+    <mergeCell ref="C128:F128"/>
+    <mergeCell ref="B142:N142"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.320138888888889" top="0.5" bottom="0.559722222222222" header="0.511805555555555" footer="0.3"/>

</xml_diff>